<commit_message>
fix(MSE-1120): Fix <td> child recursion.
</commit_message>
<xml_diff>
--- a/tests/fixtures/templates/tags/td/td.xlsx
+++ b/tests/fixtures/templates/tags/td/td.xlsx
@@ -1,87 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prateek.pisat/htmxl/tests/fixtures/templates/tags/td/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7970DB8C-AFDE-8447-981E-F1B1F93C5372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="f2c2d1de" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="7e862dbb" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Col 1</t>
-  </si>
-  <si>
-    <t>Col 2</t>
-  </si>
-  <si>
-    <t>col 1</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="7">
+    <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
+    <font/>
+    <font>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Arial"/>
       <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
+      <b val="1"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <color rgb="FFFF0000"/>
+    </font>
+    <font>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <b val="1"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -95,17 +64,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
@@ -114,31 +77,93 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="7"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="7"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="8"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="bold" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="bold_text_red-font" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="red-font" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="text" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="xl-centered" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="xl-underlined" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+  <cellStyles count="9">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="xl-centered" xfId="1" hidden="0"/>
+    <cellStyle name="xl-underlined" xfId="2" hidden="0"/>
+    <cellStyle name="regular" xfId="3" hidden="0"/>
+    <cellStyle name="bold" xfId="4" hidden="0"/>
+    <cellStyle name="text" xfId="5" hidden="0"/>
+    <cellStyle name="red-font" xfId="6" hidden="0"/>
+    <cellStyle name="bold_text_red-font" xfId="7" hidden="0"/>
+    <cellStyle name="bold_text" xfId="8" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -426,31 +451,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Col 1</t>
+        </is>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Col 2</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>col 1</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation sqref="B2" showErrorMessage="1" showDropDown="0" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Active,Inactive"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fix(MSE-1120): Fix <td> child recursion. (#37)
fix(MSE-1120): Fix <td> child recursion.
</commit_message>
<xml_diff>
--- a/tests/fixtures/templates/tags/td/td.xlsx
+++ b/tests/fixtures/templates/tags/td/td.xlsx
@@ -1,87 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prateek.pisat/htmxl/tests/fixtures/templates/tags/td/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7970DB8C-AFDE-8447-981E-F1B1F93C5372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="f2c2d1de" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="7e862dbb" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Col 1</t>
-  </si>
-  <si>
-    <t>Col 2</t>
-  </si>
-  <si>
-    <t>col 1</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="7">
+    <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
+    <font/>
+    <font>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Arial"/>
       <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
+      <b val="1"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <color rgb="FFFF0000"/>
+    </font>
+    <font>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <b val="1"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -95,17 +64,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
@@ -114,31 +77,93 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="7"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="7"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="8"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="bold" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="bold_text_red-font" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="red-font" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="text" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="xl-centered" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="xl-underlined" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+  <cellStyles count="9">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="xl-centered" xfId="1" hidden="0"/>
+    <cellStyle name="xl-underlined" xfId="2" hidden="0"/>
+    <cellStyle name="regular" xfId="3" hidden="0"/>
+    <cellStyle name="bold" xfId="4" hidden="0"/>
+    <cellStyle name="text" xfId="5" hidden="0"/>
+    <cellStyle name="red-font" xfId="6" hidden="0"/>
+    <cellStyle name="bold_text_red-font" xfId="7" hidden="0"/>
+    <cellStyle name="bold_text" xfId="8" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -426,31 +451,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Col 1</t>
+        </is>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Col 2</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>col 1</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation sqref="B2" showErrorMessage="1" showDropDown="0" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Active,Inactive"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
feat: Add support for value  attribute for input  tag.
</commit_message>
<xml_diff>
--- a/tests/fixtures/templates/tags/td/td.xlsx
+++ b/tests/fixtures/templates/tags/td/td.xlsx
@@ -1,56 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prateek.pisat/htmxl/tests/fixtures/templates/tags/td/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B41B35-3D25-9148-9C3C-65ED9B9B1DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="7e862dbb" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="7e862dbb" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Col 1</t>
+  </si>
+  <si>
+    <t>Col 2</t>
+  </si>
+  <si>
+    <t>col 1</t>
+  </si>
+  <si>
+    <t>Col 3</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="7">
-    <font>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font/>
-    <font>
-      <u val="single"/>
-    </font>
-    <font>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
-    </font>
-    <font>
       <name val="Arial"/>
-      <b val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
-    </font>
-    <font>
       <color rgb="FFFF0000"/>
-    </font>
-    <font>
       <name val="Arial"/>
-      <b val="1"/>
-      <color rgb="FFFF0000"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -64,11 +95,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
@@ -80,90 +117,31 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="7"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="8"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="7"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="8"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="xl-centered" xfId="1" hidden="0"/>
-    <cellStyle name="xl-underlined" xfId="2" hidden="0"/>
-    <cellStyle name="regular" xfId="3" hidden="0"/>
-    <cellStyle name="bold" xfId="4" hidden="0"/>
-    <cellStyle name="text" xfId="5" hidden="0"/>
-    <cellStyle name="red-font" xfId="6" hidden="0"/>
-    <cellStyle name="bold_text_red-font" xfId="7" hidden="0"/>
-    <cellStyle name="bold_text" xfId="8" hidden="0"/>
+    <cellStyle name="bold" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="bold_text" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="bold_text_red-font" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="red-font" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="text" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="xl-centered" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="xl-underlined" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -451,41 +429,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Col 1</t>
-        </is>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Col 2</t>
-        </is>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>col 1</t>
-        </is>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="B2" showErrorMessage="1" showDropDown="0" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Active,Inactive"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add support for value attribute for input tag. (#38)
</commit_message>
<xml_diff>
--- a/tests/fixtures/templates/tags/td/td.xlsx
+++ b/tests/fixtures/templates/tags/td/td.xlsx
@@ -1,56 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prateek.pisat/htmxl/tests/fixtures/templates/tags/td/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B41B35-3D25-9148-9C3C-65ED9B9B1DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="7e862dbb" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="7e862dbb" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Col 1</t>
+  </si>
+  <si>
+    <t>Col 2</t>
+  </si>
+  <si>
+    <t>col 1</t>
+  </si>
+  <si>
+    <t>Col 3</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="7">
-    <font>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font/>
-    <font>
-      <u val="single"/>
-    </font>
-    <font>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
-    </font>
-    <font>
       <name val="Arial"/>
-      <b val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
-    </font>
-    <font>
       <color rgb="FFFF0000"/>
-    </font>
-    <font>
       <name val="Arial"/>
-      <b val="1"/>
-      <color rgb="FFFF0000"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -64,11 +95,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
@@ -80,90 +117,31 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="7"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="8"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="7"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="8"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="xl-centered" xfId="1" hidden="0"/>
-    <cellStyle name="xl-underlined" xfId="2" hidden="0"/>
-    <cellStyle name="regular" xfId="3" hidden="0"/>
-    <cellStyle name="bold" xfId="4" hidden="0"/>
-    <cellStyle name="text" xfId="5" hidden="0"/>
-    <cellStyle name="red-font" xfId="6" hidden="0"/>
-    <cellStyle name="bold_text_red-font" xfId="7" hidden="0"/>
-    <cellStyle name="bold_text" xfId="8" hidden="0"/>
+    <cellStyle name="bold" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="bold_text" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="bold_text_red-font" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="red-font" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="text" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="xl-centered" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="xl-underlined" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -451,41 +429,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Col 1</t>
-        </is>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Col 2</t>
-        </is>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>col 1</t>
-        </is>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="B2" showErrorMessage="1" showDropDown="0" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Active,Inactive"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fix(MSE-1154): Fix inline styler.
</commit_message>
<xml_diff>
--- a/tests/fixtures/templates/tags/td/td.xlsx
+++ b/tests/fixtures/templates/tags/td/td.xlsx
@@ -1,87 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prateek.pisat/htmxl/tests/fixtures/templates/tags/td/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B41B35-3D25-9148-9C3C-65ED9B9B1DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="7e862dbb" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="24b3b3f3" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Col 1</t>
-  </si>
-  <si>
-    <t>Col 2</t>
-  </si>
-  <si>
-    <t>col 1</t>
-  </si>
-  <si>
-    <t>Col 3</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="7">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font/>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <u val="single"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <b val="1"/>
       <sz val="10"/>
-      <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <color rgb="FFFF0000"/>
     </font>
     <font>
-      <sz val="11"/>
+      <name val="Arial"/>
+      <b val="1"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -95,17 +64,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
@@ -117,31 +80,90 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="7"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="8"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="7"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="8"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="bold" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="bold_text" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="bold_text_red-font" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="red-font" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="text" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="xl-centered" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="xl-underlined" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="xl-centered" xfId="1" hidden="0"/>
+    <cellStyle name="xl-underlined" xfId="2" hidden="0"/>
+    <cellStyle name="regular" xfId="3" hidden="0"/>
+    <cellStyle name="bold" xfId="4" hidden="0"/>
+    <cellStyle name="text" xfId="5" hidden="0"/>
+    <cellStyle name="red-font" xfId="6" hidden="0"/>
+    <cellStyle name="bold_text_red-font" xfId="7" hidden="0"/>
+    <cellStyle name="bold_text" xfId="8" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -429,37 +451,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Col 1</t>
+        </is>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Col 2</t>
+        </is>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Col 3</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>col 1</t>
+        </is>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C2" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation sqref="B2 C2" showErrorMessage="1" showDropDown="0" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Active,Inactive"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fix(MSE-1154): Fix inline styler. (#40)
</commit_message>
<xml_diff>
--- a/tests/fixtures/templates/tags/td/td.xlsx
+++ b/tests/fixtures/templates/tags/td/td.xlsx
@@ -1,87 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prateek.pisat/htmxl/tests/fixtures/templates/tags/td/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B41B35-3D25-9148-9C3C-65ED9B9B1DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="7e862dbb" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="24b3b3f3" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Col 1</t>
-  </si>
-  <si>
-    <t>Col 2</t>
-  </si>
-  <si>
-    <t>col 1</t>
-  </si>
-  <si>
-    <t>Col 3</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="7">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font/>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <u val="single"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <b val="1"/>
       <sz val="10"/>
-      <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <color rgb="FFFF0000"/>
     </font>
     <font>
-      <sz val="11"/>
+      <name val="Arial"/>
+      <b val="1"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -95,17 +64,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
@@ -117,31 +80,90 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="7"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="8"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="7"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="8"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="bold" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="bold_text" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="bold_text_red-font" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="red-font" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="text" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="xl-centered" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="xl-underlined" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="xl-centered" xfId="1" hidden="0"/>
+    <cellStyle name="xl-underlined" xfId="2" hidden="0"/>
+    <cellStyle name="regular" xfId="3" hidden="0"/>
+    <cellStyle name="bold" xfId="4" hidden="0"/>
+    <cellStyle name="text" xfId="5" hidden="0"/>
+    <cellStyle name="red-font" xfId="6" hidden="0"/>
+    <cellStyle name="bold_text_red-font" xfId="7" hidden="0"/>
+    <cellStyle name="bold_text" xfId="8" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -429,37 +451,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Col 1</t>
+        </is>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Col 2</t>
+        </is>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Col 3</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>col 1</t>
+        </is>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C2" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation sqref="B2 C2" showErrorMessage="1" showDropDown="0" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Active,Inactive"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>